<commit_message>
Added to project management file
</commit_message>
<xml_diff>
--- a/management/project description.xlsx
+++ b/management/project description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owenpetchey/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samross/Documents/GitHub/multifarious_response_diversity/management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4512EDA-95DC-1D45-8ADF-DBAAF8E23440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F387BFA9-D984-744F-AE59-181A6BFEF0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="720" windowWidth="29080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="720" windowWidth="29080" windowHeight="19260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fundamentals" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>First name</t>
   </si>
@@ -223,6 +227,18 @@
   </si>
   <si>
     <t>Making and resporting a measure of response diversity that can handle multifarious environmental change</t>
+  </si>
+  <si>
+    <t>0000-0001-9402-9119</t>
+  </si>
+  <si>
+    <t>SamRoss</t>
+  </si>
+  <si>
+    <t>If I end up finding a useful empirical dataset…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: not really sure my contributions to this project warrant authorship (so far at least!) </t>
   </si>
 </sst>
 </file>
@@ -308,21 +324,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -644,86 +656,86 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="14.5" style="7"/>
+    <col min="1" max="1" width="21.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="14.5" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -745,11 +757,11 @@
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -844,7 +856,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -870,7 +882,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -929,7 +941,9 @@
       <c r="B5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D5" s="5" t="str">
         <f>_xlfn.CONCAT(A5,B5)</f>
         <v>SamRoss</v>
@@ -964,10 +978,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -976,7 +990,7 @@
     <col min="2" max="2" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -984,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -992,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1000,7 +1014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1008,7 +1022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1024,7 +1038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1040,7 +1054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1056,12 +1070,42 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1148,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Diversity in z completed
</commit_message>
<xml_diff>
--- a/management/project description.xlsx
+++ b/management/project description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samross/Documents/GitHub/multifarious_response_diversity/management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesco/Documents/GitHub/multifarious_response_diversity/management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F387BFA9-D984-744F-AE59-181A6BFEF0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B03DA41-E157-9C41-9ECE-1AD3FD98A5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="720" windowWidth="29080" windowHeight="19260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="720" windowWidth="37440" windowHeight="24040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fundamentals" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>First name</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">NB: not really sure my contributions to this project warrant authorship (so far at least!) </t>
+  </si>
+  <si>
+    <t>0000-0003-2092-5011</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -856,7 +859,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -911,7 +914,9 @@
       <c r="B3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="D3" s="5" t="str">
         <f>_xlfn.CONCAT(A3,B3)</f>
         <v>PolazzoFrancesco</v>
@@ -978,10 +983,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1106,6 +1111,46 @@
       </c>
       <c r="C14" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>